<commit_message>
Revised transcriptions (e.g., name verifications, 9 to 5, 9bre to Dbre)
</commit_message>
<xml_diff>
--- a/data/transcriptions/transcription_ex1.xlsx
+++ b/data/transcriptions/transcription_ex1.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/serenekim/Library/CloudStorage/OneDrive-VrijeUniversiteitBrussel/img-analysis_seorin_project/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/seorin_kim_vub_be/Documents/img-analysis_seorin_project/data/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89EA9A68-0CFC-C247-B25A-C939E897A082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{89EA9A68-0CFC-C247-B25A-C939E897A082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7221401E-6C14-BE47-A5F8-FBD92A7DEBC9}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{6D6EFBF4-D3F9-A04D-9AC4-202B897D114E}"/>
+    <workbookView xWindow="15760" yWindow="760" windowWidth="14480" windowHeight="18880" xr2:uid="{6D6EFBF4-D3F9-A04D-9AC4-202B897D114E}"/>
   </bookViews>
   <sheets>
     <sheet name="IMG_2024_03_19_11_45_57_427" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +40,6 @@
   <authors>
     <author>tc={F6329581-67FE-D446-9D65-3B6FA85C28B6}</author>
     <author>tc={93412397-27B7-ED45-B9E8-56E2B888678C}</author>
-    <author>tc={A418FE72-27AF-4D42-A32D-D0976AD90BAD}</author>
   </authors>
   <commentList>
     <comment ref="K2" authorId="0" shapeId="0" xr:uid="{F6329581-67FE-D446-9D65-3B6FA85C28B6}">
@@ -59,14 +58,6 @@
     398 part 2</t>
       </text>
     </comment>
-    <comment ref="B6" authorId="2" shapeId="0" xr:uid="{A418FE72-27AF-4D42-A32D-D0976AD90BAD}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    ditto</t>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -173,9 +164,6 @@
     <t>Herrent Maris &amp; autres</t>
   </si>
   <si>
-    <t>11 9b 1919</t>
-  </si>
-  <si>
     <t>15 7bre 1919</t>
   </si>
   <si>
@@ -200,9 +188,6 @@
     <t>Areolie Therése</t>
   </si>
   <si>
-    <t>234/1919</t>
-  </si>
-  <si>
     <t xml:space="preserve">arreté le premier novembre 1919 </t>
   </si>
   <si>
@@ -248,9 +233,6 @@
     <t>Willock Elise &amp; autres</t>
   </si>
   <si>
-    <t>15 9b 1919</t>
-  </si>
-  <si>
     <t>18 mars 1921</t>
   </si>
   <si>
@@ -281,9 +263,6 @@
     <t>Bouty Marie &amp; Gélin</t>
   </si>
   <si>
-    <t>26 9b 1919</t>
-  </si>
-  <si>
     <t>non passible</t>
   </si>
   <si>
@@ -305,9 +284,6 @@
     <t>Hessen Gustave</t>
   </si>
   <si>
-    <t>332/1928</t>
-  </si>
-  <si>
     <t>12 mars 1919</t>
   </si>
   <si>
@@ -327,6 +303,21 @@
   </si>
   <si>
     <t>Raoul Oscar</t>
+  </si>
+  <si>
+    <t>15 Db 1919</t>
+  </si>
+  <si>
+    <t>11 Db 1919</t>
+  </si>
+  <si>
+    <t>26 Db 1919</t>
+  </si>
+  <si>
+    <t>33^2/1928</t>
+  </si>
+  <si>
+    <t>214/1919</t>
   </si>
 </sst>
 </file>
@@ -893,9 +884,6 @@
   <threadedComment ref="A6" dT="2024-06-05T09:26:39.05" personId="{1AD915DC-3A0C-2F48-9C8B-C8EDAE0F9D6B}" id="{93412397-27B7-ED45-B9E8-56E2B888678C}">
     <text>398 part 2</text>
   </threadedComment>
-  <threadedComment ref="B6" dT="2024-06-05T09:57:35.10" personId="{1AD915DC-3A0C-2F48-9C8B-C8EDAE0F9D6B}" id="{A418FE72-27AF-4D42-A32D-D0976AD90BAD}">
-    <text>ditto</text>
-  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -903,8 +891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB076F5B-4564-1543-8968-7E29FE54F40E}">
   <dimension ref="A1:U15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="137" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1015,10 +1003,10 @@
       <c r="A3" s="6"/>
       <c r="B3" s="4"/>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -1035,7 +1023,7 @@
       <c r="A4" s="6"/>
       <c r="B4" s="4"/>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="5"/>
@@ -1066,7 +1054,7 @@
         <v>30</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>31</v>
@@ -1086,14 +1074,14 @@
       <c r="L5" s="5"/>
       <c r="N5" s="4"/>
       <c r="O5" t="s">
+        <v>81</v>
+      </c>
+      <c r="P5" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>34</v>
       </c>
       <c r="Q5" s="5"/>
       <c r="R5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S5" s="4">
         <v>303</v>
@@ -1103,36 +1091,36 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>37</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>38</v>
-      </c>
-      <c r="E6" t="s">
-        <v>39</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>41</v>
-      </c>
       <c r="I6">
-        <v>2229</v>
+        <v>2225</v>
       </c>
       <c r="K6" s="4">
-        <v>2229</v>
+        <v>2225</v>
       </c>
       <c r="L6" s="5"/>
       <c r="M6" t="s">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="N6" s="4"/>
       <c r="P6" s="4"/>
@@ -1145,10 +1133,10 @@
       <c r="A7" s="6"/>
       <c r="B7" s="4"/>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -1165,10 +1153,10 @@
       <c r="A8" s="6"/>
       <c r="B8" s="4"/>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
@@ -1185,13 +1173,13 @@
       <c r="A9" s="6"/>
       <c r="B9" s="4"/>
       <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="E9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>45</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
@@ -1208,13 +1196,13 @@
       <c r="A10" s="6"/>
       <c r="B10" s="4"/>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
@@ -1232,23 +1220,23 @@
         <v>399</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" t="s">
         <v>52</v>
       </c>
-      <c r="C11" t="s">
+      <c r="E11" t="s">
         <v>53</v>
-      </c>
-      <c r="D11" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" t="s">
-        <v>55</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I11">
         <v>9480</v>
@@ -1262,14 +1250,14 @@
       <c r="L11" s="5"/>
       <c r="N11" s="4"/>
       <c r="O11" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="Q11" s="5"/>
       <c r="R11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="S11" s="4">
         <v>39</v>
@@ -1282,29 +1270,29 @@
         <v>400</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I12">
         <v>690510</v>
       </c>
       <c r="J12">
-        <v>21417</v>
+        <v>31417</v>
       </c>
       <c r="K12" s="4">
         <v>659093</v>
@@ -1312,10 +1300,10 @@
       <c r="L12" s="5"/>
       <c r="N12" s="4"/>
       <c r="O12" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="Q12" s="5"/>
       <c r="S12" s="4"/>
@@ -1327,23 +1315,23 @@
         <v>401</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I13">
         <v>2277</v>
@@ -1354,14 +1342,14 @@
       <c r="L13" s="5"/>
       <c r="N13" s="4"/>
       <c r="O13" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="P13" s="4" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="Q13" s="5"/>
       <c r="R13" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="S13" s="4"/>
       <c r="T13" s="5"/>
@@ -1371,10 +1359,10 @@
       <c r="A14" s="6"/>
       <c r="B14" s="4"/>
       <c r="C14" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
@@ -1392,23 +1380,23 @@
         <v>402</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F15" s="11"/>
       <c r="G15" s="13" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="I15" s="12">
         <v>17737</v>
@@ -1420,17 +1408,17 @@
       <c r="L15" s="13"/>
       <c r="M15" s="12"/>
       <c r="N15" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="O15" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="O15" s="12" t="s">
-        <v>82</v>
-      </c>
       <c r="P15" s="11" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="Q15" s="13"/>
       <c r="R15" s="12" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="S15" s="11">
         <v>82</v>

</xml_diff>

<commit_message>
remove Note from xlsx
</commit_message>
<xml_diff>
--- a/data/transcriptions/transcription_ex1.xlsx
+++ b/data/transcriptions/transcription_ex1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/seorin_kim_vub_be/Documents/img-analysis_seorin_project/data/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{89EA9A68-0CFC-C247-B25A-C939E897A082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B1ACC76-8146-DB46-8790-17622CBD9724}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="13_ncr:1_{89EA9A68-0CFC-C247-B25A-C939E897A082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9368C57-2FBD-1846-A703-A91FE6ECE0D6}"/>
   <bookViews>
-    <workbookView xWindow="16220" yWindow="760" windowWidth="14020" windowHeight="18880" xr2:uid="{6D6EFBF4-D3F9-A04D-9AC4-202B897D114E}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{6D6EFBF4-D3F9-A04D-9AC4-202B897D114E}"/>
   </bookViews>
   <sheets>
     <sheet name="IMG_2024_03_19_11_45_57_427" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
     <author>tc={93412397-27B7-ED45-B9E8-56E2B888678C}</author>
   </authors>
   <commentList>
-    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{F6329581-67FE-D446-9D65-3B6FA85C28B6}">
+    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{F6329581-67FE-D446-9D65-3B6FA85C28B6}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="84">
   <si>
     <t>Nom.</t>
   </si>
@@ -312,9 +312,6 @@
   </si>
   <si>
     <t>arreté le trois novembre 1919 servais</t>
-  </si>
-  <si>
-    <t>Note</t>
   </si>
   <si>
     <t>Date du décès ou du judgement d'envoi en possession, en cas d'absence.</t>
@@ -348,7 +345,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -455,30 +452,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -498,7 +475,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -511,17 +488,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -538,6 +513,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -878,7 +854,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="K2" dT="2024-06-04T15:34:06.38" personId="{1AD915DC-3A0C-2F48-9C8B-C8EDAE0F9D6B}" id="{F6329581-67FE-D446-9D65-3B6FA85C28B6}">
+  <threadedComment ref="J2" dT="2024-06-04T15:34:06.38" personId="{1AD915DC-3A0C-2F48-9C8B-C8EDAE0F9D6B}" id="{F6329581-67FE-D446-9D65-3B6FA85C28B6}">
     <text>Actif-passif=restant</text>
   </threadedComment>
   <threadedComment ref="A6" dT="2024-06-05T09:26:39.05" personId="{1AD915DC-3A0C-2F48-9C8B-C8EDAE0F9D6B}" id="{93412397-27B7-ED45-B9E8-56E2B888678C}">
@@ -889,154 +865,151 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB076F5B-4564-1543-8968-7E29FE54F40E}">
-  <dimension ref="A1:U15"/>
+  <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="137" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="255" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:21" ht="51" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:20" ht="51" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="H1" s="16" t="s">
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="H1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="18"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="2" t="s">
+      <c r="I1" s="16"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="L1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="15"/>
-      <c r="O1" s="14" t="s">
+      <c r="M1" s="13"/>
+      <c r="N1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="16" t="s">
+      <c r="O1" s="13"/>
+      <c r="P1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="14" t="s">
+      <c r="Q1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="15"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="T1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="204" x14ac:dyDescent="0.2">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="8" t="s">
+    <row r="2" spans="1:20" ht="204" x14ac:dyDescent="0.2">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="3" t="s">
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="I2" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="J2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="3" t="s">
+      <c r="P2" s="15"/>
+      <c r="Q2" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="R2" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="S2" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="U2" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" s="17"/>
       <c r="B3" s="4"/>
-      <c r="F3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>76</v>
       </c>
+      <c r="F3" s="5"/>
       <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="5"/>
-      <c r="N3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="5"/>
-      <c r="S3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="5"/>
+      <c r="M3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="5"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="5"/>
       <c r="T3" s="5"/>
-      <c r="U3" s="5"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A4" s="5"/>
       <c r="B4" s="4"/>
-      <c r="F4" t="s">
+      <c r="C4" t="s">
         <v>77</v>
       </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="5"/>
       <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="5"/>
-      <c r="N4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="5"/>
-      <c r="S4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="5"/>
+      <c r="M4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="5"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="5"/>
       <c r="T4" s="5"/>
-      <c r="U4" s="5"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A5" s="6">
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
         <v>398</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -1051,42 +1024,41 @@
       <c r="E5" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="4"/>
+      <c r="F5" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="G5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5" s="5" t="s">
         <v>31</v>
       </c>
+      <c r="H5">
+        <v>2280</v>
+      </c>
       <c r="I5">
-        <v>2280</v>
-      </c>
-      <c r="J5">
         <v>1045</v>
       </c>
-      <c r="K5" s="4">
+      <c r="J5" s="4">
         <v>1235</v>
       </c>
-      <c r="L5" s="5"/>
-      <c r="N5" s="4"/>
-      <c r="O5" t="s">
+      <c r="K5" s="5"/>
+      <c r="M5" s="4"/>
+      <c r="N5" t="s">
         <v>72</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="O5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="Q5" s="5"/>
-      <c r="R5" t="s">
+      <c r="P5" s="5"/>
+      <c r="Q5" t="s">
         <v>33</v>
       </c>
-      <c r="S5" s="4">
+      <c r="R5" s="4">
         <v>303</v>
       </c>
+      <c r="S5" s="5"/>
       <c r="T5" s="5"/>
-      <c r="U5" s="5"/>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
         <v>34</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -1101,106 +1073,105 @@
       <c r="E6" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="4"/>
+      <c r="F6" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="G6" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="I6">
+      <c r="H6">
         <v>2225</v>
       </c>
-      <c r="K6" s="4">
+      <c r="J6" s="4">
         <v>2225</v>
       </c>
-      <c r="L6" s="5"/>
-      <c r="M6" t="s">
+      <c r="K6" s="5"/>
+      <c r="L6" t="s">
         <v>75</v>
       </c>
-      <c r="N6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="5"/>
-      <c r="S6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="5"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="5"/>
       <c r="T6" s="5"/>
-      <c r="U6" s="5"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
       <c r="B7" s="4"/>
-      <c r="F7" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>78</v>
       </c>
+      <c r="F7" s="5"/>
       <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="5"/>
-      <c r="N7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="5"/>
-      <c r="S7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="5"/>
+      <c r="M7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="5"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="5"/>
       <c r="T7" s="5"/>
-      <c r="U7" s="5"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
       <c r="B8" s="4"/>
-      <c r="F8" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>79</v>
       </c>
+      <c r="F8" s="5"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="5"/>
-      <c r="N8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="5"/>
-      <c r="S8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="5"/>
+      <c r="M8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="5"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="5"/>
       <c r="T8" s="5"/>
-      <c r="U8" s="5"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
       <c r="B9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>80</v>
+      </c>
       <c r="E9" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>80</v>
-      </c>
+      <c r="F9" s="5"/>
       <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="5"/>
-      <c r="N9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="5"/>
-      <c r="S9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="5"/>
+      <c r="M9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="5"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="5"/>
       <c r="T9" s="5"/>
-      <c r="U9" s="5"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A10" s="5"/>
       <c r="B10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>81</v>
+      </c>
       <c r="E10" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>81</v>
-      </c>
+      <c r="F10" s="5"/>
       <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="5"/>
-      <c r="N10" s="4"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="5"/>
-      <c r="S10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="5"/>
+      <c r="M10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="5"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="5"/>
       <c r="T10" s="5"/>
-      <c r="U10" s="5"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A11" s="6">
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
         <v>399</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -1212,45 +1183,44 @@
       <c r="D11" t="s">
         <v>44</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4" t="s">
+      <c r="F11" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="G11" s="5" t="s">
         <v>47</v>
       </c>
+      <c r="H11">
+        <v>9480</v>
+      </c>
       <c r="I11">
-        <v>9480</v>
-      </c>
-      <c r="J11">
         <v>530</v>
       </c>
-      <c r="K11" s="4">
+      <c r="J11" s="4">
         <v>8950</v>
       </c>
-      <c r="L11" s="5"/>
-      <c r="N11" s="4"/>
-      <c r="O11" t="s">
+      <c r="K11" s="5"/>
+      <c r="M11" s="4"/>
+      <c r="N11" t="s">
         <v>71</v>
       </c>
-      <c r="P11" s="4" t="s">
+      <c r="O11" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="Q11" s="5"/>
-      <c r="R11" t="s">
+      <c r="P11" s="5"/>
+      <c r="Q11" t="s">
         <v>49</v>
       </c>
-      <c r="S11" s="4">
+      <c r="R11" s="4">
         <v>39</v>
       </c>
+      <c r="S11" s="5"/>
       <c r="T11" s="5"/>
-      <c r="U11" s="5"/>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A12" s="6">
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
         <v>400</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -1259,43 +1229,42 @@
       <c r="C12" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="8" t="s">
         <v>70</v>
       </c>
       <c r="E12" t="s">
         <v>51</v>
       </c>
-      <c r="F12" s="4"/>
+      <c r="F12" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="G12" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="H12" s="5" t="s">
         <v>53</v>
       </c>
+      <c r="H12">
+        <v>690510</v>
+      </c>
       <c r="I12">
-        <v>690510</v>
-      </c>
-      <c r="J12">
         <v>31417</v>
       </c>
-      <c r="K12" s="4">
+      <c r="J12" s="4">
         <v>659093</v>
       </c>
-      <c r="L12" s="5"/>
-      <c r="N12" s="4"/>
-      <c r="O12" t="s">
+      <c r="K12" s="5"/>
+      <c r="M12" s="4"/>
+      <c r="N12" t="s">
         <v>67</v>
       </c>
-      <c r="P12" s="4" t="s">
+      <c r="O12" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="Q12" s="5"/>
-      <c r="S12" s="4"/>
+      <c r="P12" s="5"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="5"/>
       <c r="T12" s="5"/>
-      <c r="U12" s="5"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A13" s="6">
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
         <v>401</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -1310,115 +1279,113 @@
       <c r="E13" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="4"/>
+      <c r="F13" s="5" t="s">
+        <v>56</v>
+      </c>
       <c r="G13" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="H13" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="I13">
+      <c r="H13">
         <v>2277</v>
       </c>
-      <c r="K13" s="4">
+      <c r="J13" s="4">
         <v>2277</v>
       </c>
-      <c r="L13" s="5"/>
-      <c r="N13" s="4"/>
-      <c r="O13" t="s">
+      <c r="K13" s="5"/>
+      <c r="M13" s="4"/>
+      <c r="N13" t="s">
         <v>67</v>
       </c>
-      <c r="P13" s="4" t="s">
+      <c r="O13" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="Q13" s="5"/>
-      <c r="R13" t="s">
+      <c r="P13" s="5"/>
+      <c r="Q13" t="s">
         <v>58</v>
       </c>
-      <c r="S13" s="4"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="5"/>
       <c r="T13" s="5"/>
-      <c r="U13" s="5"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A14" s="5"/>
       <c r="B14" s="4"/>
-      <c r="F14" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>82</v>
       </c>
+      <c r="F14" s="5"/>
       <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="5"/>
-      <c r="N14" s="4"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="5"/>
-      <c r="S14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="5"/>
+      <c r="M14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="5"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="5"/>
       <c r="T14" s="5"/>
-      <c r="U14" s="5"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A15" s="10">
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A15" s="11">
         <v>402</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F15" s="11"/>
-      <c r="G15" s="13" t="s">
+      <c r="F15" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="H15" s="13" t="s">
+      <c r="G15" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="I15" s="12">
+      <c r="H15" s="10">
         <v>17737</v>
       </c>
-      <c r="J15" s="12"/>
-      <c r="K15" s="11">
+      <c r="I15" s="10"/>
+      <c r="J15" s="9">
         <v>17737</v>
       </c>
-      <c r="L15" s="13"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="11" t="s">
+      <c r="K15" s="11"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="O15" s="12" t="s">
+      <c r="N15" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="P15" s="11" t="s">
+      <c r="O15" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="Q15" s="13"/>
-      <c r="R15" s="12" t="s">
+      <c r="P15" s="11"/>
+      <c r="Q15" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="S15" s="11">
+      <c r="R15" s="9">
         <v>82</v>
       </c>
-      <c r="T15" s="13"/>
-      <c r="U15" s="13"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:R1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="H1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>